<commit_message>
Fix value read of text-cells on percent-formated cells
</commit_message>
<xml_diff>
--- a/tests/data/text_in_percent_cell.xlsx
+++ b/tests/data/text_in_percent_cell.xlsx
@@ -20,9 +20,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
     <t xml:space="preserve">bla</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bla with text</t>
+  </si>
+  <si>
+    <t xml:space="preserve">text</t>
   </si>
 </sst>
 </file>
@@ -123,25 +129,31 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:A6"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="11.52"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="2" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="2" min="1" style="1" width="11.52"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="3" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="n">
         <v>1</v>
       </c>
     </row>
@@ -149,20 +161,37 @@
       <c r="A3" s="1" t="n">
         <v>0.232</v>
       </c>
+      <c r="B3" s="1" t="n">
+        <v>0.232</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="n">
         <v>0.01</v>
       </c>
+      <c r="B4" s="1" t="n">
+        <v>0.01</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="n">
         <v>0.1</v>
       </c>
+      <c r="B5" s="1" t="n">
+        <v>0.1</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="n">
         <v>1</v>
+      </c>
+      <c r="B6" s="1" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B7" s="1" t="s">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>